<commit_message>
add LICENSE file and new PDF documents for overlay functionality
</commit_message>
<xml_diff>
--- a/highlight_xlsx/highlight_xlsx.xlsx
+++ b/highlight_xlsx/highlight_xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\matu\work\ToDo\easypdf\highlight_pdf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\matu\work\ToDo\easypdf\highlight_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8940DDF0-A723-429D-B3CD-EA8FA23A5322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D7AE4F-3EC4-43A1-8E0A-BDFD8BD2DB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28965" yWindow="4545" windowWidth="16410" windowHeight="20745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>